<commit_message>
Corretti errori casi test ID 24, 25, 26, 27
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-VPS/V.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-VPS/V.2.0/report-checklist.xlsx
@@ -314,10 +314,10 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>852bb807e7e5673d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.4aeb1400ff27df85f80ae99b3e0378e094fb2d308c71361f42a5899cb81a99a5.914fee2415^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>92f5e031b5d59d9a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.4aeb1400ff27df85f80ae99b3e0378e094fb2d308c71361f42a5899cb81a99a5.b02151eaf1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -334,10 +334,10 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>59e7f60e449ca5d0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.4aeb1400ff27df85f80ae99b3e0378e094fb2d308c71361f42a5899cb81a99a5.4ed60e9a27^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>0352b3c3ff3c165e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.4aeb1400ff27df85f80ae99b3e0378e094fb2d308c71361f42a5899cb81a99a5.342c59bb6b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT3</t>
@@ -348,10 +348,10 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>820c1d3d9e18862b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.4aeb1400ff27df85f80ae99b3e0378e094fb2d308c71361f42a5899cb81a99a5.f5740134d7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>b03511f8370cf3ae</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.4aeb1400ff27df85f80ae99b3e0378e094fb2d308c71361f42a5899cb81a99a5.c219a064f4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT4</t>
@@ -362,10 +362,10 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>c81aa954b1b2c92b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.140.4.4.4aeb1400ff27df85f80ae99b3e0378e094fb2d308c71361f42a5899cb81a99a5.cd14e8f078^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>c9c8af8608f6f65e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.140.4.4.4aeb1400ff27df85f80ae99b3e0378e094fb2d308c71361f42a5899cb81a99a5.ee54a8eb07^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_VPS_KO</t>
@@ -1685,19 +1685,25 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1710,9 +1716,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1732,9 +1735,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3468,10 +3468,10 @@
         <v>47</v>
       </c>
       <c r="F10" s="47">
-        <v>45012</v>
+        <v>45028</v>
       </c>
       <c r="G10" s="48">
-        <v>1679922170</v>
+        <v>1681309152</v>
       </c>
       <c r="H10" t="s" s="49">
         <v>48</v>
@@ -3512,10 +3512,10 @@
         <v>53</v>
       </c>
       <c r="F11" s="47">
-        <v>45012</v>
+        <v>45028</v>
       </c>
       <c r="G11" s="48">
-        <v>1679922704</v>
+        <v>1681309205</v>
       </c>
       <c r="H11" t="s" s="49">
         <v>54</v>
@@ -3556,10 +3556,10 @@
         <v>57</v>
       </c>
       <c r="F12" s="47">
-        <v>45012</v>
+        <v>45028</v>
       </c>
       <c r="G12" s="48">
-        <v>1679923100</v>
+        <v>1681309592</v>
       </c>
       <c r="H12" t="s" s="49">
         <v>58</v>
@@ -3599,16 +3599,16 @@
       <c r="E13" t="s" s="46">
         <v>61</v>
       </c>
-      <c r="F13" s="47">
-        <v>45013</v>
-      </c>
-      <c r="G13" s="48">
-        <v>1680008851</v>
-      </c>
-      <c r="H13" t="s" s="49">
+      <c r="F13" s="55">
+        <v>45028</v>
+      </c>
+      <c r="G13" s="56">
+        <v>1681309645</v>
+      </c>
+      <c r="H13" t="s" s="57">
         <v>62</v>
       </c>
-      <c r="I13" t="s" s="49">
+      <c r="I13" t="s" s="57">
         <v>63</v>
       </c>
       <c r="J13" t="s" s="50">
@@ -3640,17 +3640,17 @@
       <c r="D14" t="s" s="45">
         <v>64</v>
       </c>
-      <c r="E14" t="s" s="55">
+      <c r="E14" t="s" s="58">
         <v>65</v>
       </c>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
       <c r="J14" t="s" s="50">
         <v>66</v>
       </c>
-      <c r="K14" t="s" s="56">
+      <c r="K14" t="s" s="60">
         <v>67</v>
       </c>
       <c r="L14" s="52"/>
@@ -3678,38 +3678,38 @@
       <c r="D15" t="s" s="45">
         <v>69</v>
       </c>
-      <c r="E15" t="s" s="55">
+      <c r="E15" t="s" s="58">
         <v>70</v>
       </c>
-      <c r="F15" s="57">
+      <c r="F15" s="55">
         <v>45014</v>
       </c>
-      <c r="G15" s="58">
+      <c r="G15" s="61">
         <v>1680076800</v>
       </c>
-      <c r="H15" t="s" s="59">
+      <c r="H15" t="s" s="57">
         <v>71</v>
       </c>
-      <c r="I15" t="s" s="59">
+      <c r="I15" t="s" s="57">
         <v>72</v>
       </c>
       <c r="J15" t="s" s="50">
         <v>50</v>
       </c>
-      <c r="K15" s="60"/>
+      <c r="K15" s="62"/>
       <c r="L15" t="s" s="50">
         <v>50</v>
       </c>
       <c r="M15" t="s" s="50">
         <v>66</v>
       </c>
-      <c r="N15" t="s" s="61">
+      <c r="N15" t="s" s="63">
         <v>73</v>
       </c>
       <c r="O15" t="s" s="50">
         <v>50</v>
       </c>
-      <c r="P15" t="s" s="56">
+      <c r="P15" t="s" s="60">
         <v>74</v>
       </c>
       <c r="Q15" s="52"/>
@@ -3735,23 +3735,23 @@
       <c r="E16" t="s" s="46">
         <v>76</v>
       </c>
-      <c r="F16" s="62">
+      <c r="F16" s="64">
         <v>45013</v>
       </c>
-      <c r="G16" s="63">
+      <c r="G16" s="65">
         <v>1680008851</v>
       </c>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
       <c r="J16" t="s" s="50">
         <v>50</v>
       </c>
       <c r="K16" s="51"/>
       <c r="L16" s="52"/>
       <c r="M16" s="52"/>
-      <c r="N16" s="60"/>
+      <c r="N16" s="62"/>
       <c r="O16" s="52"/>
-      <c r="P16" t="s" s="65">
+      <c r="P16" t="s" s="66">
         <v>77</v>
       </c>
       <c r="Q16" s="52"/>
@@ -3779,10 +3779,10 @@
       <c r="E17" t="s" s="46">
         <v>79</v>
       </c>
-      <c r="F17" s="64">
+      <c r="F17" s="59">
         <v>45013</v>
       </c>
-      <c r="G17" s="66">
+      <c r="G17" s="67">
         <v>1680008526</v>
       </c>
       <c r="H17" t="s" s="49">
@@ -3807,7 +3807,7 @@
       <c r="O17" t="s" s="50">
         <v>66</v>
       </c>
-      <c r="P17" t="s" s="61">
+      <c r="P17" t="s" s="63">
         <v>83</v>
       </c>
       <c r="Q17" s="52"/>
@@ -3861,7 +3861,7 @@
       <c r="O18" t="s" s="50">
         <v>66</v>
       </c>
-      <c r="P18" t="s" s="67">
+      <c r="P18" t="s" s="68">
         <v>89</v>
       </c>
       <c r="Q18" s="52"/>
@@ -4239,7 +4239,7 @@
       <c r="O25" t="s" s="50">
         <v>66</v>
       </c>
-      <c r="P25" t="s" s="61">
+      <c r="P25" t="s" s="63">
         <v>131</v>
       </c>
       <c r="Q25" s="52"/>
@@ -4293,7 +4293,7 @@
       <c r="O26" t="s" s="50">
         <v>66</v>
       </c>
-      <c r="P26" t="s" s="67">
+      <c r="P26" t="s" s="68">
         <v>137</v>
       </c>
       <c r="Q26" s="52"/>
@@ -5060,54 +5060,54 @@
       </c>
     </row>
     <row r="41" ht="105.05" customHeight="1">
-      <c r="A41" s="68">
+      <c r="A41" s="69">
         <v>146</v>
       </c>
-      <c r="B41" t="s" s="69">
+      <c r="B41" t="s" s="70">
         <v>44</v>
       </c>
-      <c r="C41" t="s" s="69">
+      <c r="C41" t="s" s="70">
         <v>45</v>
       </c>
-      <c r="D41" t="s" s="69">
+      <c r="D41" t="s" s="70">
         <v>220</v>
       </c>
-      <c r="E41" t="s" s="70">
+      <c r="E41" t="s" s="71">
         <v>221</v>
       </c>
-      <c r="F41" s="57">
+      <c r="F41" s="55">
         <v>45013</v>
       </c>
-      <c r="G41" s="71">
+      <c r="G41" s="56">
         <v>1680006606</v>
       </c>
-      <c r="H41" t="s" s="59">
+      <c r="H41" t="s" s="57">
         <v>222</v>
       </c>
-      <c r="I41" t="s" s="59">
+      <c r="I41" t="s" s="57">
         <v>223</v>
       </c>
-      <c r="J41" t="s" s="61">
+      <c r="J41" t="s" s="63">
         <v>50</v>
       </c>
       <c r="K41" s="72"/>
-      <c r="L41" t="s" s="61">
+      <c r="L41" t="s" s="63">
         <v>50</v>
       </c>
-      <c r="M41" t="s" s="61">
+      <c r="M41" t="s" s="63">
         <v>50</v>
       </c>
-      <c r="N41" t="s" s="61">
+      <c r="N41" t="s" s="63">
         <v>224</v>
       </c>
-      <c r="O41" t="s" s="61">
+      <c r="O41" t="s" s="63">
         <v>66</v>
       </c>
-      <c r="P41" t="s" s="61">
+      <c r="P41" t="s" s="63">
         <v>225</v>
       </c>
       <c r="Q41" s="73"/>
-      <c r="R41" s="61"/>
+      <c r="R41" s="63"/>
       <c r="S41" s="74"/>
       <c r="T41" t="s" s="75">
         <v>68</v>

</xml_diff>